<commit_message>
admin ver. 1.0 beta
-add new car
-modification car
</commit_message>
<xml_diff>
--- a/CarRentPlanner.xlsx
+++ b/CarRentPlanner.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
   <si>
     <t xml:space="preserve">Cars</t>
   </si>
@@ -204,7 +204,45 @@
     <t xml:space="preserve">modCar</t>
   </si>
   <si>
-    <t xml:space="preserve">Modificationcar.html</t>
+    <t xml:space="preserve">selectioncar.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/admin/cars/mod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CarId::int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autó kiválasztása szerkesztésre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificationcar.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CarDto::CarDTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/admin/cars/new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateNumber::Sring
+Type::String
+Price::int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">új autó hozzáadása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/admin/cars/mod/modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateNumber::Sring
+Type::String
+Price::int
+Active::boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autó módosítása</t>
   </si>
   <si>
     <t xml:space="preserve">Név</t>
@@ -255,7 +293,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -278,14 +315,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -293,14 +328,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="4">
@@ -382,7 +415,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -451,12 +484,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -573,16 +618,16 @@
         <a:srgbClr val="0000ff"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -590,67 +635,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -669,35 +672,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -1912,15 +1891,15 @@
   </sheetPr>
   <dimension ref="A1:G988"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="25.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="30.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="28.89"/>
@@ -2043,7 +2022,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -2066,7 +2045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
         <v>50</v>
       </c>
@@ -2089,32 +2068,98 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="11" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3122,31 +3167,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>39</v>
@@ -3154,10 +3199,10 @@
     </row>
     <row r="5" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>